<commit_message>
Third Day 1st push, scrapped site for countries completed
</commit_message>
<xml_diff>
--- a/data/total players by country.xlsx
+++ b/data/total players by country.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\J2das\Documents\NSS\PYTHON\Projects\NSS-Full-Time-Data-Analytics-14-Capstone-Dota2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{980CE812-D412-474A-BF87-E9CA41E5BFBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34A785A-79E8-4F15-B329-879297D07AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14715" yWindow="0" windowWidth="13275" windowHeight="12780" xr2:uid="{E8132CEB-F6DD-4FD9-8A20-A34A9B4C2D37}"/>
+    <workbookView xWindow="11325" yWindow="165" windowWidth="13275" windowHeight="12780" xr2:uid="{E8132CEB-F6DD-4FD9-8A20-A34A9B4C2D37}"/>
   </bookViews>
   <sheets>
     <sheet name="Countries 2014" sheetId="1" r:id="rId1"/>
@@ -113,45 +113,6 @@
     <t>South Korea</t>
   </si>
   <si>
-    <t>TI 2011</t>
-  </si>
-  <si>
-    <t>TI 2012</t>
-  </si>
-  <si>
-    <t>TI 2013</t>
-  </si>
-  <si>
-    <t>TI 2014</t>
-  </si>
-  <si>
-    <t>TI 2015</t>
-  </si>
-  <si>
-    <t>TI 2016</t>
-  </si>
-  <si>
-    <t>TI 2017</t>
-  </si>
-  <si>
-    <t>TI 2018</t>
-  </si>
-  <si>
-    <t>TI 2019</t>
-  </si>
-  <si>
-    <t>TI 2021</t>
-  </si>
-  <si>
-    <t>TI 2022</t>
-  </si>
-  <si>
-    <t>TI 2023</t>
-  </si>
-  <si>
-    <t>TI 2024</t>
-  </si>
-  <si>
     <t>Finalnd</t>
   </si>
   <si>
@@ -234,6 +195,45 @@
   </si>
   <si>
     <t>Nicaragua</t>
+  </si>
+  <si>
+    <t>ti2011</t>
+  </si>
+  <si>
+    <t>ti2012</t>
+  </si>
+  <si>
+    <t>ti2013</t>
+  </si>
+  <si>
+    <t>ti2014</t>
+  </si>
+  <si>
+    <t>ti2015</t>
+  </si>
+  <si>
+    <t>ti2016</t>
+  </si>
+  <si>
+    <t>ti2017</t>
+  </si>
+  <si>
+    <t>ti2018</t>
+  </si>
+  <si>
+    <t>ti2019</t>
+  </si>
+  <si>
+    <t>ti2021</t>
+  </si>
+  <si>
+    <t>ti2022</t>
+  </si>
+  <si>
+    <t>ti2023</t>
+  </si>
+  <si>
+    <t>ti2024</t>
   </si>
 </sst>
 </file>
@@ -607,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EB0CFF2-4565-426D-85FF-A1AAF4D714B8}">
   <dimension ref="B2:AA34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="Z29" sqref="Z29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -635,79 +635,79 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="F2" t="s">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>27</v>
+        <v>55</v>
       </c>
       <c r="H2" t="s">
         <v>0</v>
       </c>
       <c r="I2" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="J2" t="s">
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="L2" t="s">
         <v>0</v>
       </c>
       <c r="M2" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="N2" t="s">
         <v>0</v>
       </c>
       <c r="O2" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="P2" t="s">
         <v>0</v>
       </c>
       <c r="Q2" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="R2" t="s">
         <v>0</v>
       </c>
       <c r="S2" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="T2" t="s">
         <v>0</v>
       </c>
       <c r="U2" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="V2" t="s">
         <v>0</v>
       </c>
       <c r="W2" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="X2" t="s">
         <v>0</v>
       </c>
       <c r="Y2" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="Z2" t="s">
         <v>0</v>
       </c>
       <c r="AA2" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="2:27" x14ac:dyDescent="0.25">
@@ -772,7 +772,7 @@
         <v>22</v>
       </c>
       <c r="V3" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="W3">
         <v>13</v>
@@ -834,7 +834,7 @@
         <v>11</v>
       </c>
       <c r="P4" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="Q4">
         <v>8</v>
@@ -846,7 +846,7 @@
         <v>9</v>
       </c>
       <c r="T4" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="U4">
         <v>10</v>
@@ -858,7 +858,7 @@
         <v>13</v>
       </c>
       <c r="X4" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="Y4">
         <v>15</v>
@@ -908,7 +908,7 @@
         <v>6</v>
       </c>
       <c r="N5" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="O5">
         <v>5</v>
@@ -944,7 +944,7 @@
         <v>9</v>
       </c>
       <c r="Z5" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="AA5">
         <v>7</v>
@@ -1006,7 +1006,7 @@
         <v>5</v>
       </c>
       <c r="T6" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="U6">
         <v>6</v>
@@ -1018,7 +1018,7 @@
         <v>8</v>
       </c>
       <c r="X6" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="Y6">
         <v>6</v>
@@ -1074,7 +1074,7 @@
         <v>5</v>
       </c>
       <c r="P7" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="Q7">
         <v>4</v>
@@ -1184,7 +1184,7 @@
         <v>4</v>
       </c>
       <c r="Z8" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="AA8">
         <v>3</v>
@@ -1264,7 +1264,7 @@
         <v>4</v>
       </c>
       <c r="Z9" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="AA9">
         <v>3</v>
@@ -1400,7 +1400,7 @@
         <v>3</v>
       </c>
       <c r="R11" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="S11">
         <v>4</v>
@@ -1412,13 +1412,13 @@
         <v>3</v>
       </c>
       <c r="V11" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="W11">
         <v>3</v>
       </c>
       <c r="X11" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="Y11">
         <v>3</v>
@@ -1572,7 +1572,7 @@
         <v>2</v>
       </c>
       <c r="V13" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="W13">
         <v>3</v>
@@ -1584,7 +1584,7 @@
         <v>3</v>
       </c>
       <c r="Z13" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="AA13">
         <v>2</v>
@@ -1604,7 +1604,7 @@
         <v>3</v>
       </c>
       <c r="F14" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -1622,7 +1622,7 @@
         <v>1</v>
       </c>
       <c r="L14" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="M14">
         <v>2</v>
@@ -1646,7 +1646,7 @@
         <v>2</v>
       </c>
       <c r="T14" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="U14">
         <v>2</v>
@@ -1696,7 +1696,7 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="K15">
         <v>1</v>
@@ -1720,7 +1720,7 @@
         <v>2</v>
       </c>
       <c r="R15" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="S15">
         <v>2</v>
@@ -1800,7 +1800,7 @@
         <v>2</v>
       </c>
       <c r="R16" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="S16">
         <v>2</v>
@@ -1856,7 +1856,7 @@
         <v>1</v>
       </c>
       <c r="L17" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="M17">
         <v>1</v>
@@ -1868,13 +1868,13 @@
         <v>2</v>
       </c>
       <c r="P17" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="Q17">
         <v>2</v>
       </c>
       <c r="R17" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="S17">
         <v>2</v>
@@ -1892,13 +1892,13 @@
         <v>2</v>
       </c>
       <c r="X17" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="Y17">
         <v>2</v>
       </c>
       <c r="Z17" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="AA17">
         <v>1</v>
@@ -1936,13 +1936,13 @@
         <v>1</v>
       </c>
       <c r="N18" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="O18">
         <v>2</v>
       </c>
       <c r="P18" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="Q18">
         <v>1</v>
@@ -1954,7 +1954,7 @@
         <v>2</v>
       </c>
       <c r="T18" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="U18">
         <v>1</v>
@@ -2004,7 +2004,7 @@
         <v>1</v>
       </c>
       <c r="N19" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="O19">
         <v>1</v>
@@ -2016,13 +2016,13 @@
         <v>1</v>
       </c>
       <c r="R19" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="S19">
         <v>1</v>
       </c>
       <c r="T19" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="U19">
         <v>1</v>
@@ -2034,13 +2034,13 @@
         <v>2</v>
       </c>
       <c r="X19" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="Y19">
         <v>2</v>
       </c>
       <c r="Z19" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="AA19">
         <v>1</v>
@@ -2054,7 +2054,7 @@
         <v>1</v>
       </c>
       <c r="J20" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="K20">
         <v>1</v>
@@ -2066,7 +2066,7 @@
         <v>1</v>
       </c>
       <c r="N20" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="O20">
         <v>1</v>
@@ -2078,13 +2078,13 @@
         <v>1</v>
       </c>
       <c r="R20" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="S20">
         <v>1</v>
       </c>
       <c r="T20" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="U20">
         <v>1</v>
@@ -2096,13 +2096,13 @@
         <v>1</v>
       </c>
       <c r="X20" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y20">
+        <v>2</v>
+      </c>
+      <c r="Z20" t="s">
         <v>49</v>
-      </c>
-      <c r="Y20">
-        <v>2</v>
-      </c>
-      <c r="Z20" t="s">
-        <v>62</v>
       </c>
       <c r="AA20">
         <v>1</v>
@@ -2116,25 +2116,25 @@
         <v>1</v>
       </c>
       <c r="J21" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="K21">
         <v>1</v>
       </c>
       <c r="L21" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="M21">
         <v>1</v>
       </c>
       <c r="N21" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="O21">
         <v>1</v>
       </c>
       <c r="P21" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="Q21">
         <v>1</v>
@@ -2152,19 +2152,19 @@
         <v>1</v>
       </c>
       <c r="V21" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="W21">
         <v>1</v>
       </c>
       <c r="X21" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="Y21">
         <v>1</v>
       </c>
       <c r="Z21" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="AA21">
         <v>1</v>
@@ -2178,7 +2178,7 @@
         <v>1</v>
       </c>
       <c r="L22" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="M22">
         <v>1</v>
@@ -2208,13 +2208,13 @@
         <v>1</v>
       </c>
       <c r="V22" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="W22">
         <v>1</v>
       </c>
       <c r="X22" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="Y22">
         <v>1</v>
@@ -2234,13 +2234,13 @@
         <v>1</v>
       </c>
       <c r="N23" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="O23">
         <v>1</v>
       </c>
       <c r="P23" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="Q23">
         <v>1</v>
@@ -2258,19 +2258,19 @@
         <v>1</v>
       </c>
       <c r="V23" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="W23">
         <v>1</v>
       </c>
       <c r="X23" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="Y23">
         <v>1</v>
       </c>
       <c r="Z23" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="AA23">
         <v>1</v>
@@ -2284,7 +2284,7 @@
         <v>1</v>
       </c>
       <c r="N24" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="O24">
         <v>1</v>
@@ -2296,7 +2296,7 @@
         <v>1</v>
       </c>
       <c r="R24" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="S24">
         <v>1</v>
@@ -2308,7 +2308,7 @@
         <v>1</v>
       </c>
       <c r="V24" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="W24">
         <v>1</v>
@@ -2320,7 +2320,7 @@
         <v>1</v>
       </c>
       <c r="Z24" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="AA24">
         <v>1</v>
@@ -2340,13 +2340,13 @@
         <v>1</v>
       </c>
       <c r="R25" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="S25">
         <v>1</v>
       </c>
       <c r="T25" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="U25">
         <v>1</v>
@@ -2372,7 +2372,7 @@
     </row>
     <row r="26" spans="2:27" x14ac:dyDescent="0.25">
       <c r="N26" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="O26">
         <v>1</v>
@@ -2384,13 +2384,13 @@
         <v>1</v>
       </c>
       <c r="R26" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="S26">
         <v>1</v>
       </c>
       <c r="T26" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="U26">
         <v>1</v>
@@ -2402,13 +2402,13 @@
         <v>1</v>
       </c>
       <c r="X26" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="Y26">
         <v>1</v>
       </c>
       <c r="Z26" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="AA26">
         <v>1</v>
@@ -2416,25 +2416,25 @@
     </row>
     <row r="27" spans="2:27" x14ac:dyDescent="0.25">
       <c r="N27" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="O27">
         <v>1</v>
       </c>
       <c r="R27" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="S27">
         <v>1</v>
       </c>
       <c r="T27" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="U27">
         <v>1</v>
       </c>
       <c r="V27" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="W27">
         <v>1</v>
@@ -2454,25 +2454,25 @@
     </row>
     <row r="28" spans="2:27" x14ac:dyDescent="0.25">
       <c r="R28" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="S28">
         <v>1</v>
       </c>
       <c r="T28" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="U28">
         <v>1</v>
       </c>
       <c r="V28" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="W28">
         <v>1</v>
       </c>
       <c r="X28" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="Y28">
         <v>1</v>
@@ -2492,13 +2492,13 @@
         <v>1</v>
       </c>
       <c r="T29" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="U29">
         <v>1</v>
       </c>
       <c r="V29" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="W29">
         <v>1</v>
@@ -2524,13 +2524,13 @@
         <v>1</v>
       </c>
       <c r="V30" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="W30">
         <v>1</v>
       </c>
       <c r="X30" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="Y30">
         <v>1</v>
@@ -2544,7 +2544,7 @@
         <v>1</v>
       </c>
       <c r="V31" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="W31">
         <v>1</v>
@@ -2558,7 +2558,7 @@
         <v>1</v>
       </c>
       <c r="V32" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="W32">
         <v>1</v>

</xml_diff>

<commit_message>
Third Day 2nd push, collected data and started to clean it
</commit_message>
<xml_diff>
--- a/data/total players by country.xlsx
+++ b/data/total players by country.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\J2das\Documents\NSS\PYTHON\Projects\NSS-Full-Time-Data-Analytics-14-Capstone-Dota2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A34A785A-79E8-4F15-B329-879297D07AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00E1F926-C7A2-4869-A4A4-E3A2623720E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11325" yWindow="165" windowWidth="13275" windowHeight="12780" xr2:uid="{E8132CEB-F6DD-4FD9-8A20-A34A9B4C2D37}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8132CEB-F6DD-4FD9-8A20-A34A9B4C2D37}"/>
   </bookViews>
   <sheets>
     <sheet name="Countries 2014" sheetId="1" r:id="rId1"/>

</xml_diff>